<commit_message>
Two columns are removed from excel hence from preprocessor too. Excel instructions are also updated
</commit_message>
<xml_diff>
--- a/Config_Exp2.xlsx
+++ b/Config_Exp2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\docs-tez-depo\ThesisWork\ANCAT\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\Github\ANCAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B24E80-48D2-466F-8DF6-6A3FF9C7CB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F722AAE-B0A1-4767-B9F2-5D1A0207DBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3408" windowWidth="19896" windowHeight="8340" activeTab="3" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
   <si>
     <t>ES1</t>
   </si>
@@ -1705,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570773CE-9739-4C1A-9F1C-7A7BF1E7D7C1}">
-  <dimension ref="A1:O88"/>
+  <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="K1" activeCellId="1" sqref="I1:I1048576 K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1721,17 +1721,15 @@
     <col min="6" max="6" width="10.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="4"/>
+    <col min="9" max="9" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="32" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="32" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>38</v>
       </c>
@@ -1757,28 +1755,22 @@
         <v>31</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1803,29 +1795,23 @@
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="4">
+      <c r="I2" s="4">
         <v>1183</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="K2" s="4">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="4">
-        <v>15000</v>
-      </c>
-      <c r="N2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1850,29 +1836,23 @@
       <c r="H3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="I3" s="4">
         <v>1183</v>
       </c>
+      <c r="J3" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="K3" s="4">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="4">
-        <v>15000</v>
-      </c>
-      <c r="N3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1897,29 +1877,23 @@
       <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="I4" s="4">
         <v>1183</v>
       </c>
+      <c r="J4" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="K4" s="4">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="4">
-        <v>15000</v>
-      </c>
-      <c r="N4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1944,50 +1918,44 @@
       <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="I5" s="4">
         <v>1183</v>
       </c>
+      <c r="J5" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="K5" s="4">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="4">
-        <v>15000</v>
-      </c>
-      <c r="N5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:15" s="3" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="3" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="D13" s="7"/>
@@ -2000,10 +1968,8 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:15" s="3" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:13" s="3" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="D14" s="7"/>
@@ -2016,10 +1982,8 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:15" s="3" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:13" s="3" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="D15" s="7"/>
@@ -2032,10 +1996,8 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
     </row>
     <row r="17" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>